<commit_message>
Commit Borrador Matriz Interaccion
</commit_message>
<xml_diff>
--- a/PrimerBorrador_Checklist.xlsx
+++ b/PrimerBorrador_Checklist.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\ProyectoMetodologia\proyectometodologia7342\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F733B01F-5213-4C92-93C1-F77959E72902}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26B1EADF-E49A-4457-9D63-532F0C342C4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{66FCFBC5-0291-4609-A468-4F8468BC42F6}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="22">
   <si>
     <t>Requisito</t>
   </si>
@@ -58,9 +58,6 @@
     <t>Observaciones</t>
   </si>
   <si>
-    <t>RQ2:El sistema debe permitir ingresar la información del registro del cliente y almacenar en un sistema de persistencia de datos</t>
-  </si>
-  <si>
     <t>RQ4: El sistema debe permitir ingresar la información del registro del trabajador y almacenar en un sistema de persistencia de datos</t>
   </si>
   <si>
@@ -73,9 +70,6 @@
     <t>no</t>
   </si>
   <si>
-    <t>Se debe especificar que informacion se debe registrar en el cliente.</t>
-  </si>
-  <si>
     <t>Se debe especificar que informacion se debe registrar en el trabajador.</t>
   </si>
   <si>
@@ -98,6 +92,12 @@
   </si>
   <si>
     <t>RQ7: El sistema debe crear una factura a partir de los productos vendidos al cliente. La información colocada en la factura debe incluir nombres completos, cédula de identidad, correo electrónico, dirección de vivienda, y teléfono, así como los datos de la empresa: dirección del establecimiento, numero del telefono celular,ruc,nombre del trabajador y un desglose de los productos que el cliente compró. Se debe considerar el 12% del IVA en cada factura.</t>
+  </si>
+  <si>
+    <t>RQ2:El sistema debe permitir almacenar la información del cliente ya ingresada en la computadora</t>
+  </si>
+  <si>
+    <t xml:space="preserve">si </t>
   </si>
 </sst>
 </file>
@@ -538,8 +538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F24A3371-B552-49DB-8C90-07F078E5FB0F}">
   <dimension ref="B2:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -582,207 +582,205 @@
         <v>7</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="2:10" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="2:10" ht="45" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>11</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>12</v>
+        <v>21</v>
+      </c>
+      <c r="I4" s="3"/>
+      <c r="J4" s="7" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="2:10" ht="78" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="2:10" ht="45" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="E6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="J6" s="6" t="s">
         <v>11</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="7" spans="2:10" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="G7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J7" s="6" t="s">
         <v>11</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J7" s="6" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="8" spans="2:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="2:10" ht="166.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="2:2" ht="45" x14ac:dyDescent="0.25">
       <c r="B17" s="8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>